<commit_message>
Reorganize code and adjust to integrate log and config table update functions
</commit_message>
<xml_diff>
--- a/fake_config_tables/water_quality_configuration_table.xlsx
+++ b/fake_config_tables/water_quality_configuration_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\program_documents\cmp_hiring\intern\2023_rachel\projects\cmp\deployment_change_tracking\deployment_change_code\updatess\fake_config_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBE277CE-856C-428C-BC0A-D4D1028E83F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F61F39-5102-4E01-8D4E-3AF0A32357BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,7 +199,7 @@
     <t>Drag Anchor Coordinates: 45.50130, -61.04167</t>
   </si>
   <si>
-    <t>Drag Anchor WP# 105: 45.50156, -61.04188_x000D__x000D_
+    <t>Drag Anchor WP# 105: 45.50156, -61.04188_x000D__x000D__x000D_
 April 2020 - Leeway unable to locate dragline</t>
   </si>
   <si>
@@ -233,7 +233,7 @@
     <t>Vertical Chain of 4 HOBOs, 2 DOTs</t>
   </si>
   <si>
-    <t>Vertical Chain of 4 HOBOs, 3 DOTs_x000D__x000D_
+    <t>Vertical Chain of 4 HOBOs, 3 DOTs_x000D__x000D__x000D_
  Evidence of drag by ice. Further search with side scan planned</t>
   </si>
   <si>
@@ -357,7 +357,7 @@
     <t>Upon download of data saw that logging stopped on 2018-06-13. Upon further investigation this was due to filling up memory (64 kb). This is due to incorrect config of 1 min logging interval instead of 1 hr interval.</t>
   </si>
   <si>
-    <t>String retreived and data were retrieved from the sensors.Redeployed back at falling tide.100% marine growth on the bigger float and about 80% on the small float with the sensors._x000D__x000D_
+    <t>String retreived and data were retrieved from the sensors.Redeployed back at falling tide.100% marine growth on the bigger float and about 80% on the small float with the sensors._x000D__x000D__x000D_
 Batteries and canister were replaced.</t>
   </si>
   <si>
@@ -589,7 +589,7 @@
     <t>Drag Anchor: 45.60285, -60.90180</t>
   </si>
   <si>
-    <t>Drag Anchor WP#108: 45.60274, -60.90325_x000D__x000D_
+    <t>Drag Anchor WP#108: 45.60274, -60.90325_x000D__x000D__x000D_
 April 2020 - Leeway unable to locate dragline</t>
   </si>
   <si>
@@ -809,8 +809,8 @@
     <t>Mackerel Island</t>
   </si>
   <si>
-    <t>Whale Sanctuary Scoping Project - Drag Anchor @44.4629, -63.67788_x000D__x000D_
-Attempted recovery by T. Balch, M. Hatcher failed_x000D__x000D_
+    <t>Whale Sanctuary Scoping Project - Drag Anchor @44.4629, -63.67788_x000D__x000D__x000D_
+Attempted recovery by T. Balch, M. Hatcher failed_x000D__x000D__x000D_
 Leeway attempted recovery August 17th 2021 - failed. Hooked onto something heavy, 500lbs+.</t>
   </si>
   <si>
@@ -847,7 +847,7 @@
     <t>New firmware (2.0.19). New Battery.</t>
   </si>
   <si>
-    <t>Retrieve and redeployed. High tide going out, 1.93m. 3 HOBOs, 1 DOT, VR2AR_x000D__x000D_
+    <t>Retrieve and redeployed. High tide going out, 1.93m. 3 HOBOs, 1 DOT, VR2AR_x000D__x000D__x000D_
 Recovered in fishermans gear - returned to DFA via DFO - Nov 4, 2021</t>
   </si>
   <si>
@@ -992,7 +992,7 @@
     <t>Outer Island</t>
   </si>
   <si>
-    <t>Drag Anchor @ 43.46897, -65.73985. _x000D__x000D_
+    <t>Drag Anchor @ 43.46897, -65.73985. _x000D__x000D__x000D_
 01/09/2020 - retrieval attempted unsuccessfully. Risk of losing grapple to other moorings. Equipment may still be present</t>
   </si>
   <si>
@@ -1011,7 +1011,7 @@
     <t>Piper Lake</t>
   </si>
   <si>
-    <t xml:space="preserve">Hobo 0.38 m above bottom, Dot 0.46 m above bottom, Drag anchor at N45.34644 W62.66084_x000D__x000D_
+    <t xml:space="preserve">Hobo 0.38 m above bottom, Dot 0.46 m above bottom, Drag anchor at N45.34644 W62.66084_x000D__x000D__x000D_
 </t>
   </si>
   <si>
@@ -1755,7 +1755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
(Partially) integrate log renaming and archiving code with station name change function
</commit_message>
<xml_diff>
--- a/fake_config_tables/water_quality_configuration_table.xlsx
+++ b/fake_config_tables/water_quality_configuration_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\program_documents\cmp_hiring\intern\2023_rachel\projects\cmp\deployment_change_tracking\deployment_change_code\updatess\fake_config_tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F61F39-5102-4E01-8D4E-3AF0A32357BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C36BE4B-8DB6-45BE-BAB6-89C57B8AE2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -199,7 +199,7 @@
     <t>Drag Anchor Coordinates: 45.50130, -61.04167</t>
   </si>
   <si>
-    <t>Drag Anchor WP# 105: 45.50156, -61.04188_x000D__x000D__x000D_
+    <t>Drag Anchor WP# 105: 45.50156, -61.04188_x000D__x000D__x000D__x000D__x000D__x000D_
 April 2020 - Leeway unable to locate dragline</t>
   </si>
   <si>
@@ -233,7 +233,7 @@
     <t>Vertical Chain of 4 HOBOs, 2 DOTs</t>
   </si>
   <si>
-    <t>Vertical Chain of 4 HOBOs, 3 DOTs_x000D__x000D__x000D_
+    <t>Vertical Chain of 4 HOBOs, 3 DOTs_x000D__x000D__x000D__x000D__x000D__x000D_
  Evidence of drag by ice. Further search with side scan planned</t>
   </si>
   <si>
@@ -357,7 +357,7 @@
     <t>Upon download of data saw that logging stopped on 2018-06-13. Upon further investigation this was due to filling up memory (64 kb). This is due to incorrect config of 1 min logging interval instead of 1 hr interval.</t>
   </si>
   <si>
-    <t>String retreived and data were retrieved from the sensors.Redeployed back at falling tide.100% marine growth on the bigger float and about 80% on the small float with the sensors._x000D__x000D__x000D_
+    <t>String retreived and data were retrieved from the sensors.Redeployed back at falling tide.100% marine growth on the bigger float and about 80% on the small float with the sensors._x000D__x000D__x000D__x000D__x000D__x000D_
 Batteries and canister were replaced.</t>
   </si>
   <si>
@@ -589,7 +589,7 @@
     <t>Drag Anchor: 45.60285, -60.90180</t>
   </si>
   <si>
-    <t>Drag Anchor WP#108: 45.60274, -60.90325_x000D__x000D__x000D_
+    <t>Drag Anchor WP#108: 45.60274, -60.90325_x000D__x000D__x000D__x000D__x000D__x000D_
 April 2020 - Leeway unable to locate dragline</t>
   </si>
   <si>
@@ -809,8 +809,8 @@
     <t>Mackerel Island</t>
   </si>
   <si>
-    <t>Whale Sanctuary Scoping Project - Drag Anchor @44.4629, -63.67788_x000D__x000D__x000D_
-Attempted recovery by T. Balch, M. Hatcher failed_x000D__x000D__x000D_
+    <t>Whale Sanctuary Scoping Project - Drag Anchor @44.4629, -63.67788_x000D__x000D__x000D__x000D__x000D__x000D_
+Attempted recovery by T. Balch, M. Hatcher failed_x000D__x000D__x000D__x000D__x000D__x000D_
 Leeway attempted recovery August 17th 2021 - failed. Hooked onto something heavy, 500lbs+.</t>
   </si>
   <si>
@@ -847,7 +847,7 @@
     <t>New firmware (2.0.19). New Battery.</t>
   </si>
   <si>
-    <t>Retrieve and redeployed. High tide going out, 1.93m. 3 HOBOs, 1 DOT, VR2AR_x000D__x000D__x000D_
+    <t>Retrieve and redeployed. High tide going out, 1.93m. 3 HOBOs, 1 DOT, VR2AR_x000D__x000D__x000D__x000D__x000D__x000D_
 Recovered in fishermans gear - returned to DFA via DFO - Nov 4, 2021</t>
   </si>
   <si>
@@ -992,7 +992,7 @@
     <t>Outer Island</t>
   </si>
   <si>
-    <t>Drag Anchor @ 43.46897, -65.73985. _x000D__x000D__x000D_
+    <t>Drag Anchor @ 43.46897, -65.73985. _x000D__x000D__x000D__x000D__x000D__x000D_
 01/09/2020 - retrieval attempted unsuccessfully. Risk of losing grapple to other moorings. Equipment may still be present</t>
   </si>
   <si>
@@ -1011,7 +1011,7 @@
     <t>Piper Lake</t>
   </si>
   <si>
-    <t xml:space="preserve">Hobo 0.38 m above bottom, Dot 0.46 m above bottom, Drag anchor at N45.34644 W62.66084_x000D__x000D__x000D_
+    <t xml:space="preserve">Hobo 0.38 m above bottom, Dot 0.46 m above bottom, Drag anchor at N45.34644 W62.66084_x000D__x000D__x000D__x000D__x000D__x000D_
 </t>
   </si>
   <si>
@@ -1755,8 +1755,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>